<commit_message>
LMSYS Chatbot Arena Leaderboard
</commit_message>
<xml_diff>
--- a/meta/Foundation Model Leaderboard Systems.xlsx
+++ b/meta/Foundation Model Leaderboard Systems.xlsx
@@ -2252,7 +2252,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2374" uniqueCount="984">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2377" uniqueCount="986">
   <si>
     <t>Leaderboard name</t>
   </si>
@@ -4807,7 +4807,7 @@
     <t>https://huggingface.co/spaces/gaia-benchmark/leaderboard/discussions/14</t>
   </si>
   <si>
-    <t>Participatory Model</t>
+    <t>Participative Model</t>
   </si>
   <si>
     <t>https://huggingface.co/spaces/opencompass/open_vlm_leaderboard/discussions/6</t>
@@ -5093,6 +5093,9 @@
     <t>https://github.com/stanford-crfm/helm/issues/2038</t>
   </si>
   <si>
+    <t>https://huggingface.co/spaces/Vchitect/VBench/discussions/1</t>
+  </si>
+  <si>
     <t>https://github.com/THU-KEG/KoLA/issues/6</t>
   </si>
   <si>
@@ -5115,6 +5118,9 @@
   </si>
   <si>
     <t>https://huggingface.co/spaces/PingAndPasquale/MOE-LLM-GPU-Poor-Leaderboard/discussions/2</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/FinancialSupport/open_ita_llm_leaderboard/discussions/6</t>
   </si>
   <si>
     <t>https://huggingface.co/spaces/PatronusAI/enterprise_scenarios_leaderboard/discussions/10</t>
@@ -9589,7 +9595,9 @@
       <c r="A188" s="8" t="s">
         <v>415</v>
       </c>
-      <c r="C188" s="2"/>
+      <c r="C188" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="D188" s="2" t="s">
         <v>416</v>
       </c>
@@ -46846,18 +46854,23 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="8" t="s">
+        <v>939</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="2" t="s">
         <v>847</v>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" s="8" t="s">
-        <v>939</v>
-      </c>
-    </row>
     <row r="10">
-      <c r="A10" s="16" t="s">
+      <c r="A10" s="8" t="s">
         <v>940</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="16" t="s">
+        <v>941</v>
       </c>
     </row>
   </sheetData>
@@ -46867,10 +46880,11 @@
     <hyperlink r:id="rId3" ref="A4"/>
     <hyperlink r:id="rId4" ref="A6"/>
     <hyperlink r:id="rId5" ref="A7"/>
-    <hyperlink r:id="rId6" ref="A9"/>
+    <hyperlink r:id="rId6" ref="A8"/>
     <hyperlink r:id="rId7" ref="A10"/>
+    <hyperlink r:id="rId8" ref="A11"/>
   </hyperlinks>
-  <drawing r:id="rId8"/>
+  <drawing r:id="rId9"/>
 </worksheet>
 </file>
 
@@ -46891,32 +46905,32 @@
     </row>
     <row r="2">
       <c r="A2" s="8" t="s">
-        <v>941</v>
+        <v>942</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="8" t="s">
-        <v>942</v>
+        <v>943</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="8" t="s">
-        <v>943</v>
+        <v>944</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="16" t="s">
-        <v>944</v>
+        <v>945</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="8" t="s">
-        <v>945</v>
+        <v>946</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="16" t="s">
-        <v>946</v>
+        <v>947</v>
       </c>
     </row>
     <row r="8">
@@ -46925,208 +46939,213 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="16" t="s">
-        <v>947</v>
+      <c r="A9" s="8" t="s">
+        <v>948</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="16" t="s">
-        <v>948</v>
+        <v>949</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="16" t="s">
-        <v>949</v>
+        <v>950</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="16" t="s">
-        <v>950</v>
+        <v>951</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="8" t="s">
-        <v>951</v>
+      <c r="A13" s="16" t="s">
+        <v>952</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="16" t="s">
-        <v>952</v>
+      <c r="A14" s="8" t="s">
+        <v>953</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="8" t="s">
-        <v>953</v>
+      <c r="A15" s="16" t="s">
+        <v>954</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="16" t="s">
-        <v>954</v>
+      <c r="A16" s="8" t="s">
+        <v>955</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="16" t="s">
-        <v>955</v>
+        <v>956</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="16" t="s">
-        <v>956</v>
+        <v>957</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="16" t="s">
-        <v>957</v>
+        <v>958</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="2" t="s">
+      <c r="A20" s="16" t="s">
+        <v>959</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="2" t="s">
         <v>870</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="8" t="s">
-        <v>958</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="8" t="s">
-        <v>959</v>
+        <v>960</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="8" t="s">
-        <v>960</v>
+        <v>961</v>
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="16" t="s">
-        <v>961</v>
+      <c r="A24" s="8" t="s">
+        <v>962</v>
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="2" t="s">
+      <c r="A25" s="16" t="s">
+        <v>963</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="2" t="s">
         <v>824</v>
       </c>
     </row>
-    <row r="26">
-      <c r="A26" s="16" t="s">
-        <v>962</v>
-      </c>
-    </row>
     <row r="27">
-      <c r="A27" s="2" t="s">
+      <c r="A27" s="16" t="s">
+        <v>964</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="2" t="s">
         <v>831</v>
       </c>
     </row>
-    <row r="28">
-      <c r="A28" s="8" t="s">
-        <v>963</v>
-      </c>
-    </row>
     <row r="29">
-      <c r="A29" s="16" t="s">
-        <v>964</v>
+      <c r="A29" s="8" t="s">
+        <v>965</v>
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="8" t="s">
-        <v>965</v>
+      <c r="A30" s="16" t="s">
+        <v>966</v>
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="2" t="s">
+      <c r="A31" s="8" t="s">
+        <v>967</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="2" t="s">
         <v>847</v>
       </c>
     </row>
-    <row r="32">
-      <c r="A32" s="8" t="s">
-        <v>966</v>
-      </c>
-    </row>
     <row r="33">
-      <c r="A33" s="16" t="s">
-        <v>967</v>
+      <c r="A33" s="8" t="s">
+        <v>968</v>
       </c>
     </row>
     <row r="34">
-      <c r="A34" s="8" t="s">
+      <c r="A34" s="16" t="s">
+        <v>969</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="8" t="s">
         <v>882</v>
       </c>
     </row>
-    <row r="35">
-      <c r="A35" s="16" t="s">
-        <v>968</v>
-      </c>
-    </row>
     <row r="36">
-      <c r="A36" s="2" t="s">
+      <c r="A36" s="16" t="s">
+        <v>970</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="2" t="s">
         <v>849</v>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" s="16" t="s">
-        <v>969</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="16" t="s">
-        <v>970</v>
+        <v>971</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="16" t="s">
-        <v>971</v>
+        <v>972</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="16" t="s">
-        <v>972</v>
+        <v>973</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="16" t="s">
-        <v>973</v>
+        <v>974</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="16" t="s">
-        <v>974</v>
+        <v>975</v>
       </c>
     </row>
     <row r="43">
-      <c r="A43" s="8" t="s">
-        <v>975</v>
+      <c r="A43" s="16" t="s">
+        <v>976</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="8" t="s">
-        <v>976</v>
+        <v>977</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="8" t="s">
-        <v>977</v>
+        <v>978</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="8" t="s">
-        <v>978</v>
+        <v>979</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="8" t="s">
-        <v>979</v>
+        <v>980</v>
       </c>
     </row>
     <row r="48">
-      <c r="A48" s="16" t="s">
-        <v>980</v>
+      <c r="A48" s="8" t="s">
+        <v>981</v>
       </c>
     </row>
     <row r="49">
-      <c r="A49" s="8" t="s">
-        <v>981</v>
+      <c r="A49" s="16" t="s">
+        <v>982</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="8" t="s">
+        <v>983</v>
       </c>
     </row>
   </sheetData>
@@ -47148,19 +47167,19 @@
     <hyperlink r:id="rId15" ref="A17"/>
     <hyperlink r:id="rId16" ref="A18"/>
     <hyperlink r:id="rId17" ref="A19"/>
-    <hyperlink r:id="rId18" ref="A21"/>
+    <hyperlink r:id="rId18" ref="A20"/>
     <hyperlink r:id="rId19" ref="A22"/>
     <hyperlink r:id="rId20" ref="A23"/>
     <hyperlink r:id="rId21" ref="A24"/>
-    <hyperlink r:id="rId22" ref="A26"/>
-    <hyperlink r:id="rId23" ref="A28"/>
+    <hyperlink r:id="rId22" ref="A25"/>
+    <hyperlink r:id="rId23" ref="A27"/>
     <hyperlink r:id="rId24" ref="A29"/>
     <hyperlink r:id="rId25" ref="A30"/>
-    <hyperlink r:id="rId26" ref="A32"/>
+    <hyperlink r:id="rId26" ref="A31"/>
     <hyperlink r:id="rId27" ref="A33"/>
     <hyperlink r:id="rId28" ref="A34"/>
     <hyperlink r:id="rId29" ref="A35"/>
-    <hyperlink r:id="rId30" ref="A37"/>
+    <hyperlink r:id="rId30" ref="A36"/>
     <hyperlink r:id="rId31" ref="A38"/>
     <hyperlink r:id="rId32" ref="A39"/>
     <hyperlink r:id="rId33" ref="A40"/>
@@ -47173,8 +47192,9 @@
     <hyperlink r:id="rId40" ref="A47"/>
     <hyperlink r:id="rId41" ref="A48"/>
     <hyperlink r:id="rId42" ref="A49"/>
+    <hyperlink r:id="rId43" ref="A50"/>
   </hyperlinks>
-  <drawing r:id="rId43"/>
+  <drawing r:id="rId44"/>
 </worksheet>
 </file>
 
@@ -47195,7 +47215,7 @@
     </row>
     <row r="2">
       <c r="A2" s="16" t="s">
-        <v>982</v>
+        <v>984</v>
       </c>
     </row>
     <row r="3">
@@ -47205,7 +47225,7 @@
     </row>
     <row r="4">
       <c r="A4" s="16" t="s">
-        <v>983</v>
+        <v>985</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix some workflow pattern accoriding to latest reponse
</commit_message>
<xml_diff>
--- a/meta/Foundation Model Leaderboard Systems.xlsx
+++ b/meta/Foundation Model Leaderboard Systems.xlsx
@@ -2266,7 +2266,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2127" uniqueCount="906">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2130" uniqueCount="908">
   <si>
     <t>Leaderboard name</t>
   </si>
@@ -4578,6 +4578,9 @@
     <t>https://huggingface.co/spaces/gaia-benchmark/leaderboard/discussions/14</t>
   </si>
   <si>
+    <t>https://huggingface.co/spaces/openlifescienceai/open_medical_llm_leaderboard/discussions/2</t>
+  </si>
+  <si>
     <t>Participative Model</t>
   </si>
   <si>
@@ -4952,6 +4955,9 @@
   </si>
   <si>
     <t>https://huggingface.co/spaces/instructkr/LogicKor-leaderboard/discussions/4</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/livecodebench/leaderboard/discussions/1</t>
   </si>
   <si>
     <t>https://github.com/open-compass/LawBench/issues/7</t>
@@ -8668,7 +8674,7 @@
       </c>
       <c r="D177" s="2"/>
       <c r="E177" s="2">
-        <v>2.0</v>
+        <v>7.0</v>
       </c>
       <c r="F177" s="2" t="s">
         <v>173</v>
@@ -16342,37 +16348,37 @@
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="2" t="s">
+      <c r="A26" s="8" t="s">
         <v>766</v>
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="16" t="s">
+      <c r="A27" s="2" t="s">
         <v>767</v>
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="2" t="s">
+      <c r="A28" s="16" t="s">
         <v>768</v>
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="8" t="s">
+      <c r="A29" s="2" t="s">
         <v>769</v>
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="16" t="s">
+      <c r="A30" s="8" t="s">
         <v>770</v>
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="8" t="s">
+      <c r="A31" s="16" t="s">
         <v>771</v>
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="16" t="s">
+      <c r="A32" s="8" t="s">
         <v>772</v>
       </c>
     </row>
@@ -16382,7 +16388,12 @@
       </c>
     </row>
     <row r="34">
-      <c r="A34" s="19"/>
+      <c r="A34" s="16" t="s">
+        <v>774</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="19"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -16407,14 +16418,15 @@
     <hyperlink r:id="rId19" ref="A23"/>
     <hyperlink r:id="rId20" ref="A24"/>
     <hyperlink r:id="rId21" ref="A25"/>
-    <hyperlink r:id="rId22" ref="A27"/>
-    <hyperlink r:id="rId23" ref="A29"/>
+    <hyperlink r:id="rId22" ref="A26"/>
+    <hyperlink r:id="rId23" ref="A28"/>
     <hyperlink r:id="rId24" ref="A30"/>
     <hyperlink r:id="rId25" ref="A31"/>
     <hyperlink r:id="rId26" ref="A32"/>
     <hyperlink r:id="rId27" ref="A33"/>
+    <hyperlink r:id="rId28" ref="A34"/>
   </hyperlinks>
-  <drawing r:id="rId28"/>
+  <drawing r:id="rId29"/>
 </worksheet>
 </file>
 
@@ -16430,12 +16442,12 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="2" t="s">
-        <v>774</v>
+        <v>775</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="16" t="s">
-        <v>775</v>
+        <v>776</v>
       </c>
     </row>
     <row r="3">
@@ -16445,27 +16457,27 @@
     </row>
     <row r="4">
       <c r="A4" s="8" t="s">
-        <v>776</v>
+        <v>777</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="8" t="s">
-        <v>777</v>
+        <v>778</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="8" t="s">
-        <v>778</v>
+        <v>779</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="16" t="s">
-        <v>779</v>
+        <v>780</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="16" t="s">
-        <v>780</v>
+        <v>781</v>
       </c>
     </row>
   </sheetData>
@@ -16493,7 +16505,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>774</v>
+        <v>775</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -16523,7 +16535,7 @@
     </row>
     <row r="2">
       <c r="A2" s="20" t="s">
-        <v>781</v>
+        <v>782</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -16553,7 +16565,7 @@
     </row>
     <row r="3">
       <c r="A3" s="20" t="s">
-        <v>782</v>
+        <v>783</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -16613,7 +16625,7 @@
     </row>
     <row r="5">
       <c r="A5" s="20" t="s">
-        <v>783</v>
+        <v>784</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -16643,7 +16655,7 @@
     </row>
     <row r="6">
       <c r="A6" s="20" t="s">
-        <v>784</v>
+        <v>785</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -16673,7 +16685,7 @@
     </row>
     <row r="7">
       <c r="A7" s="20" t="s">
-        <v>785</v>
+        <v>786</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -16703,7 +16715,7 @@
     </row>
     <row r="8">
       <c r="A8" s="20" t="s">
-        <v>786</v>
+        <v>787</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -16733,7 +16745,7 @@
     </row>
     <row r="9">
       <c r="A9" s="20" t="s">
-        <v>787</v>
+        <v>788</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -16763,7 +16775,7 @@
     </row>
     <row r="10">
       <c r="A10" s="20" t="s">
-        <v>788</v>
+        <v>789</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -16793,7 +16805,7 @@
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>789</v>
+        <v>790</v>
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -16823,7 +16835,7 @@
     </row>
     <row r="12">
       <c r="A12" s="20" t="s">
-        <v>790</v>
+        <v>791</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -16853,7 +16865,7 @@
     </row>
     <row r="13">
       <c r="A13" s="20" t="s">
-        <v>791</v>
+        <v>792</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -16883,7 +16895,7 @@
     </row>
     <row r="14">
       <c r="A14" s="20" t="s">
-        <v>792</v>
+        <v>793</v>
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -16943,7 +16955,7 @@
     </row>
     <row r="16">
       <c r="A16" s="20" t="s">
-        <v>793</v>
+        <v>794</v>
       </c>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -16973,7 +16985,7 @@
     </row>
     <row r="17">
       <c r="A17" s="20" t="s">
-        <v>781</v>
+        <v>782</v>
       </c>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -17003,7 +17015,7 @@
     </row>
     <row r="18">
       <c r="A18" s="20" t="s">
-        <v>794</v>
+        <v>795</v>
       </c>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -17033,7 +17045,7 @@
     </row>
     <row r="19">
       <c r="A19" s="20" t="s">
-        <v>795</v>
+        <v>796</v>
       </c>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -17063,7 +17075,7 @@
     </row>
     <row r="20">
       <c r="A20" s="20" t="s">
-        <v>796</v>
+        <v>797</v>
       </c>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -17093,7 +17105,7 @@
     </row>
     <row r="21">
       <c r="A21" s="20" t="s">
-        <v>797</v>
+        <v>798</v>
       </c>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -17153,7 +17165,7 @@
     </row>
     <row r="23">
       <c r="A23" s="20" t="s">
-        <v>798</v>
+        <v>799</v>
       </c>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -17183,7 +17195,7 @@
     </row>
     <row r="24">
       <c r="A24" s="1" t="s">
-        <v>766</v>
+        <v>767</v>
       </c>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -17213,7 +17225,7 @@
     </row>
     <row r="25">
       <c r="A25" s="20" t="s">
-        <v>799</v>
+        <v>800</v>
       </c>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -17243,7 +17255,7 @@
     </row>
     <row r="26">
       <c r="A26" s="20" t="s">
-        <v>800</v>
+        <v>801</v>
       </c>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -17273,7 +17285,7 @@
     </row>
     <row r="27">
       <c r="A27" s="20" t="s">
-        <v>801</v>
+        <v>802</v>
       </c>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -17303,7 +17315,7 @@
     </row>
     <row r="28">
       <c r="A28" s="20" t="s">
-        <v>802</v>
+        <v>803</v>
       </c>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -17333,7 +17345,7 @@
     </row>
     <row r="29">
       <c r="A29" s="20" t="s">
-        <v>803</v>
+        <v>804</v>
       </c>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -17363,7 +17375,7 @@
     </row>
     <row r="30">
       <c r="A30" s="20" t="s">
-        <v>804</v>
+        <v>805</v>
       </c>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -44566,22 +44578,22 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="2" t="s">
-        <v>774</v>
+        <v>775</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="16" t="s">
-        <v>805</v>
+        <v>806</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="16" t="s">
-        <v>806</v>
+        <v>807</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="16" t="s">
-        <v>807</v>
+        <v>808</v>
       </c>
     </row>
     <row r="5">
@@ -44591,62 +44603,62 @@
     </row>
     <row r="6">
       <c r="A6" s="8" t="s">
-        <v>808</v>
+        <v>809</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="8" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="8" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="16" t="s">
-        <v>811</v>
+        <v>812</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="16" t="s">
-        <v>812</v>
+        <v>813</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="16" t="s">
-        <v>813</v>
+        <v>814</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="16" t="s">
-        <v>814</v>
+        <v>815</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="16" t="s">
-        <v>815</v>
+        <v>816</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="8" t="s">
-        <v>816</v>
+        <v>817</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="8" t="s">
-        <v>817</v>
+        <v>818</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="16" t="s">
-        <v>818</v>
+        <v>819</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="16" t="s">
-        <v>819</v>
+        <v>820</v>
       </c>
     </row>
     <row r="18">
@@ -44656,22 +44668,22 @@
     </row>
     <row r="19">
       <c r="A19" s="16" t="s">
-        <v>820</v>
+        <v>821</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="8" t="s">
-        <v>821</v>
+        <v>822</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="16" t="s">
-        <v>822</v>
+        <v>823</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="16" t="s">
-        <v>823</v>
+        <v>824</v>
       </c>
     </row>
     <row r="23">
@@ -44681,77 +44693,77 @@
     </row>
     <row r="24">
       <c r="A24" s="8" t="s">
-        <v>824</v>
+        <v>825</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="16" t="s">
-        <v>825</v>
+        <v>826</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="16" t="s">
-        <v>826</v>
+        <v>827</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="16" t="s">
-        <v>827</v>
+        <v>828</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="16" t="s">
-        <v>828</v>
+        <v>829</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="16" t="s">
-        <v>829</v>
+        <v>830</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="16" t="s">
-        <v>830</v>
+        <v>831</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="16" t="s">
-        <v>831</v>
+        <v>832</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="16" t="s">
-        <v>832</v>
+        <v>833</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="2" t="s">
-        <v>766</v>
+        <v>767</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="16" t="s">
-        <v>833</v>
+        <v>834</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="16" t="s">
-        <v>834</v>
+        <v>835</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="2" t="s">
-        <v>768</v>
+        <v>769</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="16" t="s">
-        <v>835</v>
+        <v>836</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="16" t="s">
-        <v>836</v>
+        <v>837</v>
       </c>
     </row>
   </sheetData>
@@ -44810,17 +44822,17 @@
     </row>
     <row r="2">
       <c r="A2" s="16" t="s">
-        <v>837</v>
+        <v>838</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="8" t="s">
-        <v>838</v>
+        <v>839</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="16" t="s">
-        <v>839</v>
+        <v>840</v>
       </c>
     </row>
     <row r="5">
@@ -44830,7 +44842,7 @@
     </row>
     <row r="6">
       <c r="A6" s="16" t="s">
-        <v>840</v>
+        <v>841</v>
       </c>
     </row>
     <row r="7">
@@ -44840,12 +44852,12 @@
     </row>
     <row r="8">
       <c r="A8" s="8" t="s">
-        <v>841</v>
+        <v>842</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="16" t="s">
-        <v>842</v>
+        <v>843</v>
       </c>
     </row>
     <row r="10">
@@ -44855,62 +44867,62 @@
     </row>
     <row r="11">
       <c r="A11" s="8" t="s">
-        <v>843</v>
+        <v>844</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="16" t="s">
-        <v>844</v>
+        <v>845</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="16" t="s">
-        <v>845</v>
+        <v>846</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="8" t="s">
-        <v>846</v>
+        <v>847</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="16" t="s">
-        <v>847</v>
+        <v>848</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="16" t="s">
-        <v>848</v>
+        <v>849</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="2" t="s">
-        <v>766</v>
+        <v>767</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="8" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="2" t="s">
-        <v>768</v>
+        <v>769</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="8" t="s">
-        <v>850</v>
+        <v>851</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="8" t="s">
-        <v>851</v>
+        <v>852</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="16" t="s">
-        <v>852</v>
+        <v>853</v>
       </c>
     </row>
   </sheetData>
@@ -44953,17 +44965,17 @@
     </row>
     <row r="2">
       <c r="A2" s="16" t="s">
-        <v>853</v>
+        <v>854</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="16" t="s">
-        <v>854</v>
+        <v>855</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="16" t="s">
-        <v>855</v>
+        <v>856</v>
       </c>
     </row>
     <row r="5">
@@ -44973,32 +44985,32 @@
     </row>
     <row r="6">
       <c r="A6" s="8" t="s">
-        <v>856</v>
+        <v>857</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="16" t="s">
-        <v>857</v>
+        <v>858</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="8" t="s">
-        <v>858</v>
+        <v>859</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="s">
-        <v>766</v>
+        <v>767</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="8" t="s">
-        <v>859</v>
+        <v>860</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="16" t="s">
-        <v>860</v>
+        <v>861</v>
       </c>
     </row>
   </sheetData>
@@ -45028,37 +45040,37 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="2" t="s">
-        <v>774</v>
+        <v>775</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="8" t="s">
-        <v>861</v>
+        <v>862</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="8" t="s">
-        <v>862</v>
+        <v>863</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="8" t="s">
-        <v>863</v>
+        <v>864</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="16" t="s">
-        <v>864</v>
+        <v>865</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="8" t="s">
-        <v>865</v>
+        <v>866</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="16" t="s">
-        <v>866</v>
+        <v>867</v>
       </c>
     </row>
     <row r="8">
@@ -45068,77 +45080,77 @@
     </row>
     <row r="9">
       <c r="A9" s="8" t="s">
-        <v>867</v>
+        <v>868</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="16" t="s">
-        <v>868</v>
+        <v>869</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="16" t="s">
-        <v>869</v>
+        <v>870</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="16" t="s">
-        <v>870</v>
+        <v>871</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="16" t="s">
-        <v>871</v>
+        <v>872</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="8" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="16" t="s">
-        <v>873</v>
+        <v>874</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="8" t="s">
-        <v>874</v>
+        <v>875</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="16" t="s">
-        <v>875</v>
+        <v>876</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="16" t="s">
-        <v>876</v>
+        <v>877</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="16" t="s">
-        <v>877</v>
+        <v>878</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="16" t="s">
-        <v>878</v>
+        <v>879</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="8" t="s">
-        <v>879</v>
+        <v>880</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="2" t="s">
-        <v>789</v>
+      <c r="A22" s="16" t="s">
+        <v>820</v>
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="8" t="s">
-        <v>880</v>
+      <c r="A23" s="2" t="s">
+        <v>790</v>
       </c>
     </row>
     <row r="24">
@@ -45152,78 +45164,78 @@
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="16" t="s">
+      <c r="A26" s="8" t="s">
         <v>883</v>
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="2" t="s">
+      <c r="A27" s="16" t="s">
+        <v>884</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="2" t="s">
         <v>743</v>
       </c>
     </row>
-    <row r="28">
-      <c r="A28" s="16" t="s">
-        <v>884</v>
-      </c>
-    </row>
     <row r="29">
-      <c r="A29" s="2" t="s">
+      <c r="A29" s="16" t="s">
+        <v>885</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="2" t="s">
         <v>750</v>
       </c>
     </row>
-    <row r="30">
-      <c r="A30" s="8" t="s">
-        <v>885</v>
-      </c>
-    </row>
     <row r="31">
-      <c r="A31" s="16" t="s">
+      <c r="A31" s="8" t="s">
         <v>886</v>
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="8" t="s">
+      <c r="A32" s="16" t="s">
         <v>887</v>
       </c>
     </row>
     <row r="33">
-      <c r="A33" s="2" t="s">
-        <v>766</v>
+      <c r="A33" s="8" t="s">
+        <v>888</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="8" t="s">
-        <v>888</v>
+        <v>889</v>
       </c>
     </row>
     <row r="35">
-      <c r="A35" s="16" t="s">
-        <v>889</v>
+      <c r="A35" s="2" t="s">
+        <v>767</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="8" t="s">
-        <v>801</v>
+        <v>890</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="16" t="s">
-        <v>890</v>
+        <v>891</v>
       </c>
     </row>
     <row r="38">
-      <c r="A38" s="2" t="s">
-        <v>768</v>
+      <c r="A38" s="8" t="s">
+        <v>802</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="16" t="s">
-        <v>891</v>
+        <v>892</v>
       </c>
     </row>
     <row r="40">
-      <c r="A40" s="16" t="s">
-        <v>892</v>
+      <c r="A40" s="2" t="s">
+        <v>769</v>
       </c>
     </row>
     <row r="41">
@@ -45247,12 +45259,12 @@
       </c>
     </row>
     <row r="45">
-      <c r="A45" s="8" t="s">
+      <c r="A45" s="16" t="s">
         <v>897</v>
       </c>
     </row>
     <row r="46">
-      <c r="A46" s="8" t="s">
+      <c r="A46" s="16" t="s">
         <v>898</v>
       </c>
     </row>
@@ -45272,13 +45284,23 @@
       </c>
     </row>
     <row r="50">
-      <c r="A50" s="16" t="s">
+      <c r="A50" s="8" t="s">
         <v>902</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="8" t="s">
         <v>903</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="16" t="s">
+        <v>904</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="8" t="s">
+        <v>905</v>
       </c>
     </row>
   </sheetData>
@@ -45302,20 +45324,20 @@
     <hyperlink r:id="rId17" ref="A19"/>
     <hyperlink r:id="rId18" ref="A20"/>
     <hyperlink r:id="rId19" ref="A21"/>
-    <hyperlink r:id="rId20" ref="A23"/>
+    <hyperlink r:id="rId20" ref="A22"/>
     <hyperlink r:id="rId21" ref="A24"/>
     <hyperlink r:id="rId22" ref="A25"/>
     <hyperlink r:id="rId23" ref="A26"/>
-    <hyperlink r:id="rId24" ref="A28"/>
-    <hyperlink r:id="rId25" ref="A30"/>
+    <hyperlink r:id="rId24" ref="A27"/>
+    <hyperlink r:id="rId25" ref="A29"/>
     <hyperlink r:id="rId26" ref="A31"/>
     <hyperlink r:id="rId27" ref="A32"/>
-    <hyperlink r:id="rId28" ref="A34"/>
-    <hyperlink r:id="rId29" ref="A35"/>
+    <hyperlink r:id="rId28" ref="A33"/>
+    <hyperlink r:id="rId29" ref="A34"/>
     <hyperlink r:id="rId30" ref="A36"/>
     <hyperlink r:id="rId31" ref="A37"/>
-    <hyperlink r:id="rId32" ref="A39"/>
-    <hyperlink r:id="rId33" ref="A40"/>
+    <hyperlink r:id="rId32" ref="A38"/>
+    <hyperlink r:id="rId33" ref="A39"/>
     <hyperlink r:id="rId34" ref="A41"/>
     <hyperlink r:id="rId35" ref="A42"/>
     <hyperlink r:id="rId36" ref="A43"/>
@@ -45327,8 +45349,10 @@
     <hyperlink r:id="rId42" ref="A49"/>
     <hyperlink r:id="rId43" ref="A50"/>
     <hyperlink r:id="rId44" ref="A51"/>
+    <hyperlink r:id="rId45" ref="A52"/>
+    <hyperlink r:id="rId46" ref="A53"/>
   </hyperlinks>
-  <drawing r:id="rId45"/>
+  <drawing r:id="rId47"/>
 </worksheet>
 </file>
 
@@ -45349,17 +45373,17 @@
     </row>
     <row r="2">
       <c r="A2" s="16" t="s">
-        <v>904</v>
+        <v>906</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>768</v>
+        <v>769</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="16" t="s">
-        <v>905</v>
+        <v>907</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update with latest reponses
</commit_message>
<xml_diff>
--- a/meta/Foundation Model Leaderboard Systems.xlsx
+++ b/meta/Foundation Model Leaderboard Systems.xlsx
@@ -4,14 +4,15 @@
   <workbookPr/>
   <sheets>
     <sheet state="visible" name="Leaderboard System" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="Inaccessible Component" sheetId="2" r:id="rId5"/>
-    <sheet state="visible" name="Misdisplayed Component" sheetId="3" r:id="rId6"/>
-    <sheet state="visible" name="Mismatched Component" sheetId="4" r:id="rId7"/>
-    <sheet state="visible" name="Missing Component" sheetId="5" r:id="rId8"/>
-    <sheet state="visible" name="Obsolete Component" sheetId="6" r:id="rId9"/>
-    <sheet state="visible" name="Redundant Component" sheetId="7" r:id="rId10"/>
-    <sheet state="visible" name="Unclear Component" sheetId="8" r:id="rId11"/>
-    <sheet state="visible" name="Unresponsive Component" sheetId="9" r:id="rId12"/>
+    <sheet state="visible" name="SATD" sheetId="2" r:id="rId5"/>
+    <sheet state="visible" name="Inaccessible Component" sheetId="3" r:id="rId6"/>
+    <sheet state="visible" name="Misdisplayed Component" sheetId="4" r:id="rId7"/>
+    <sheet state="visible" name="Mismatched Component" sheetId="5" r:id="rId8"/>
+    <sheet state="visible" name="Missing Component" sheetId="6" r:id="rId9"/>
+    <sheet state="visible" name="Obsolete Component" sheetId="7" r:id="rId10"/>
+    <sheet state="visible" name="Redundant Component" sheetId="8" r:id="rId11"/>
+    <sheet state="visible" name="Unclear Component" sheetId="9" r:id="rId12"/>
+    <sheet state="visible" name="Unresponsive Component" sheetId="10" r:id="rId13"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -2266,7 +2267,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2130" uniqueCount="908">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2135" uniqueCount="911">
   <si>
     <t>Leaderboard name</t>
   </si>
@@ -2286,7 +2287,7 @@
     <t>Platforms</t>
   </si>
   <si>
-    <t>Platforms with model linkage (non-pwc)</t>
+    <t>Model linkage (non-pwc)</t>
   </si>
   <si>
     <t>Publication venues</t>
@@ -4503,6 +4504,21 @@
     <t>αNLI</t>
   </si>
   <si>
+    <t>https://huggingface.co/spaces/FSMBench/Leaderboard/discussions/3</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/sparse-generative-ai/open-moe-llm-leaderboard/discussions/2</t>
+  </si>
+  <si>
+    <t>https://github.com/stanford-crfm/helm/issues/2441</t>
+  </si>
+  <si>
+    <t>https://github.com/stanford-crfm/helm/issues/2205</t>
+  </si>
+  <si>
+    <t>https://github.com/stanford-crfm/helm/issues/2351</t>
+  </si>
+  <si>
     <t>Evaluation Dataset</t>
   </si>
   <si>
@@ -4705,9 +4721,6 @@
   </si>
   <si>
     <t>https://github.com/OpenM3D/M3DBench/issues/2</t>
-  </si>
-  <si>
-    <t>https://huggingface.co/spaces/FSMBench/Leaderboard/discussions/3</t>
   </si>
   <si>
     <t>https://huggingface.co/spaces/instructkr/LogicKor-leaderboard/discussions/6</t>
@@ -4925,9 +4938,6 @@
   </si>
   <si>
     <t>https://github.com/stanford-crfm/helm/issues/2358</t>
-  </si>
-  <si>
-    <t>https://github.com/stanford-crfm/helm/issues/2441</t>
   </si>
   <si>
     <t>https://huggingface.co/spaces/malhajar/OpenLLMTurkishLeaderboard/discussions/5</t>
@@ -5169,6 +5179,10 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing10.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -16212,6 +16226,45 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="2" t="s">
+        <v>755</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="16" t="s">
+        <v>909</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="s">
+        <v>774</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="16" t="s">
+        <v>910</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink r:id="rId1" ref="A2"/>
+    <hyperlink r:id="rId2" ref="A4"/>
+  </hyperlinks>
+  <drawing r:id="rId3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
@@ -16223,7 +16276,7 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="16" t="s">
         <v>741</v>
       </c>
     </row>
@@ -16233,163 +16286,210 @@
       </c>
     </row>
     <row r="3">
+      <c r="A3" s="16" t="s">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="16" t="s">
+        <v>744</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="16" t="s">
+        <v>745</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink r:id="rId1" ref="A1"/>
+    <hyperlink r:id="rId2" ref="A2"/>
+    <hyperlink r:id="rId3" ref="A3"/>
+    <hyperlink r:id="rId4" ref="A4"/>
+    <hyperlink r:id="rId5" ref="A5"/>
+  </hyperlinks>
+  <drawing r:id="rId6"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="2" t="s">
+        <v>746</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="16" t="s">
+        <v>747</v>
+      </c>
+    </row>
+    <row r="3">
       <c r="A3" s="2" t="s">
-        <v>743</v>
+        <v>748</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="8" t="s">
-        <v>744</v>
+        <v>749</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="8" t="s">
-        <v>745</v>
+        <v>750</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="16" t="s">
-        <v>746</v>
+        <v>751</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="16" t="s">
-        <v>747</v>
+        <v>752</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="s">
-        <v>748</v>
+        <v>753</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="16" t="s">
-        <v>749</v>
+        <v>754</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="s">
-        <v>750</v>
+        <v>755</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="8" t="s">
-        <v>751</v>
+        <v>756</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="8" t="s">
-        <v>752</v>
+        <v>757</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="8" t="s">
-        <v>753</v>
+        <v>758</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="8" t="s">
-        <v>754</v>
+        <v>759</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="8" t="s">
-        <v>755</v>
+        <v>760</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="8" t="s">
-        <v>756</v>
+        <v>761</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="8" t="s">
-        <v>757</v>
+        <v>762</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="8" t="s">
-        <v>758</v>
+        <v>763</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="8" t="s">
-        <v>759</v>
+        <v>764</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="8" t="s">
-        <v>760</v>
+        <v>765</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="16" t="s">
-        <v>761</v>
+        <v>766</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="8" t="s">
-        <v>762</v>
+        <v>767</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="8" t="s">
-        <v>763</v>
+        <v>768</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="8" t="s">
-        <v>764</v>
+        <v>769</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="16" t="s">
-        <v>765</v>
+        <v>770</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="8" t="s">
-        <v>766</v>
+        <v>771</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="2" t="s">
-        <v>767</v>
+        <v>772</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="16" t="s">
-        <v>768</v>
+        <v>773</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="2" t="s">
-        <v>769</v>
+        <v>774</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="8" t="s">
-        <v>770</v>
+        <v>775</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="16" t="s">
-        <v>771</v>
+        <v>776</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="8" t="s">
-        <v>772</v>
+        <v>777</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="16" t="s">
-        <v>773</v>
+        <v>778</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="16" t="s">
-        <v>774</v>
+        <v>779</v>
       </c>
     </row>
     <row r="35">
@@ -16430,7 +16530,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -16442,42 +16542,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="2" t="s">
-        <v>775</v>
+        <v>780</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="16" t="s">
-        <v>776</v>
+        <v>781</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>750</v>
+        <v>755</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="8" t="s">
-        <v>777</v>
+        <v>782</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="8" t="s">
-        <v>778</v>
+        <v>783</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="8" t="s">
-        <v>779</v>
+        <v>784</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="16" t="s">
-        <v>780</v>
+        <v>785</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="16" t="s">
-        <v>781</v>
+        <v>786</v>
       </c>
     </row>
   </sheetData>
@@ -16493,7 +16593,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -16505,7 +16605,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>775</v>
+        <v>780</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -16535,7 +16635,7 @@
     </row>
     <row r="2">
       <c r="A2" s="20" t="s">
-        <v>782</v>
+        <v>787</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -16565,7 +16665,7 @@
     </row>
     <row r="3">
       <c r="A3" s="20" t="s">
-        <v>783</v>
+        <v>788</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -16595,7 +16695,7 @@
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>741</v>
+        <v>746</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -16625,7 +16725,7 @@
     </row>
     <row r="5">
       <c r="A5" s="20" t="s">
-        <v>784</v>
+        <v>789</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -16655,7 +16755,7 @@
     </row>
     <row r="6">
       <c r="A6" s="20" t="s">
-        <v>785</v>
+        <v>790</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -16685,7 +16785,7 @@
     </row>
     <row r="7">
       <c r="A7" s="20" t="s">
-        <v>786</v>
+        <v>791</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -16715,7 +16815,7 @@
     </row>
     <row r="8">
       <c r="A8" s="20" t="s">
-        <v>787</v>
+        <v>792</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -16745,7 +16845,7 @@
     </row>
     <row r="9">
       <c r="A9" s="20" t="s">
-        <v>788</v>
+        <v>793</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -16775,7 +16875,7 @@
     </row>
     <row r="10">
       <c r="A10" s="20" t="s">
-        <v>789</v>
+        <v>794</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -16805,7 +16905,7 @@
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>790</v>
+        <v>795</v>
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -16835,7 +16935,7 @@
     </row>
     <row r="12">
       <c r="A12" s="20" t="s">
-        <v>791</v>
+        <v>796</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -16865,7 +16965,7 @@
     </row>
     <row r="13">
       <c r="A13" s="20" t="s">
-        <v>792</v>
+        <v>797</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -16895,7 +16995,7 @@
     </row>
     <row r="14">
       <c r="A14" s="20" t="s">
-        <v>793</v>
+        <v>798</v>
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -16925,7 +17025,7 @@
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
-        <v>743</v>
+        <v>748</v>
       </c>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -16955,7 +17055,7 @@
     </row>
     <row r="16">
       <c r="A16" s="20" t="s">
-        <v>794</v>
+        <v>799</v>
       </c>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -16985,7 +17085,7 @@
     </row>
     <row r="17">
       <c r="A17" s="20" t="s">
-        <v>782</v>
+        <v>787</v>
       </c>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -17015,7 +17115,7 @@
     </row>
     <row r="18">
       <c r="A18" s="20" t="s">
-        <v>795</v>
+        <v>800</v>
       </c>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -17045,7 +17145,7 @@
     </row>
     <row r="19">
       <c r="A19" s="20" t="s">
-        <v>796</v>
+        <v>801</v>
       </c>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -17075,7 +17175,7 @@
     </row>
     <row r="20">
       <c r="A20" s="20" t="s">
-        <v>797</v>
+        <v>802</v>
       </c>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -17105,7 +17205,7 @@
     </row>
     <row r="21">
       <c r="A21" s="20" t="s">
-        <v>798</v>
+        <v>803</v>
       </c>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -17135,7 +17235,7 @@
     </row>
     <row r="22">
       <c r="A22" s="1" t="s">
-        <v>750</v>
+        <v>755</v>
       </c>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -17165,7 +17265,7 @@
     </row>
     <row r="23">
       <c r="A23" s="20" t="s">
-        <v>799</v>
+        <v>804</v>
       </c>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -17195,7 +17295,7 @@
     </row>
     <row r="24">
       <c r="A24" s="1" t="s">
-        <v>767</v>
+        <v>772</v>
       </c>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -17225,7 +17325,7 @@
     </row>
     <row r="25">
       <c r="A25" s="20" t="s">
-        <v>800</v>
+        <v>805</v>
       </c>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -17255,7 +17355,7 @@
     </row>
     <row r="26">
       <c r="A26" s="20" t="s">
-        <v>801</v>
+        <v>806</v>
       </c>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -17285,7 +17385,7 @@
     </row>
     <row r="27">
       <c r="A27" s="20" t="s">
-        <v>802</v>
+        <v>807</v>
       </c>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -17315,7 +17415,7 @@
     </row>
     <row r="28">
       <c r="A28" s="20" t="s">
-        <v>803</v>
+        <v>808</v>
       </c>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -17345,7 +17445,7 @@
     </row>
     <row r="29">
       <c r="A29" s="20" t="s">
-        <v>804</v>
+        <v>809</v>
       </c>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -17375,7 +17475,7 @@
     </row>
     <row r="30">
       <c r="A30" s="20" t="s">
-        <v>805</v>
+        <v>810</v>
       </c>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -44566,7 +44666,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -44578,192 +44678,192 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="2" t="s">
-        <v>775</v>
+        <v>780</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="16" t="s">
-        <v>806</v>
+        <v>811</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="16" t="s">
-        <v>807</v>
+        <v>812</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="16" t="s">
-        <v>808</v>
+        <v>813</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>741</v>
+        <v>746</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="8" t="s">
-        <v>809</v>
+        <v>741</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="8" t="s">
-        <v>810</v>
+        <v>814</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="8" t="s">
-        <v>811</v>
+        <v>815</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="16" t="s">
-        <v>812</v>
+        <v>816</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="16" t="s">
-        <v>813</v>
+        <v>817</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="16" t="s">
-        <v>814</v>
+        <v>818</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="16" t="s">
-        <v>815</v>
+        <v>819</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="16" t="s">
-        <v>816</v>
+        <v>820</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="8" t="s">
-        <v>817</v>
+        <v>821</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="8" t="s">
-        <v>818</v>
+        <v>822</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="16" t="s">
-        <v>819</v>
+        <v>823</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="16" t="s">
-        <v>820</v>
+        <v>824</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="2" t="s">
-        <v>743</v>
+        <v>748</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="16" t="s">
-        <v>821</v>
+        <v>825</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="8" t="s">
-        <v>822</v>
+        <v>826</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="16" t="s">
-        <v>823</v>
+        <v>827</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="16" t="s">
-        <v>824</v>
+        <v>828</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="2" t="s">
-        <v>750</v>
+        <v>755</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="8" t="s">
-        <v>825</v>
+        <v>829</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="16" t="s">
-        <v>826</v>
+        <v>830</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="16" t="s">
-        <v>827</v>
+        <v>831</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="16" t="s">
-        <v>828</v>
+        <v>832</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="16" t="s">
-        <v>829</v>
+        <v>833</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="16" t="s">
-        <v>830</v>
+        <v>834</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="16" t="s">
-        <v>831</v>
+        <v>835</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="16" t="s">
-        <v>832</v>
+        <v>836</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="16" t="s">
-        <v>833</v>
+        <v>837</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="2" t="s">
-        <v>767</v>
+        <v>772</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="16" t="s">
-        <v>834</v>
+        <v>838</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="16" t="s">
-        <v>835</v>
+        <v>839</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="2" t="s">
-        <v>769</v>
+        <v>774</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="16" t="s">
-        <v>836</v>
+        <v>840</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="16" t="s">
-        <v>837</v>
+        <v>841</v>
       </c>
     </row>
   </sheetData>
@@ -44805,7 +44905,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -44817,112 +44917,112 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="2" t="s">
-        <v>741</v>
+        <v>746</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="16" t="s">
-        <v>838</v>
+        <v>842</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="8" t="s">
-        <v>839</v>
+        <v>843</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="16" t="s">
-        <v>840</v>
+        <v>844</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>743</v>
+        <v>748</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="16" t="s">
-        <v>841</v>
+        <v>845</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="s">
-        <v>748</v>
+        <v>753</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="8" t="s">
-        <v>842</v>
+        <v>846</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="16" t="s">
-        <v>843</v>
+        <v>847</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="s">
-        <v>750</v>
+        <v>755</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="8" t="s">
-        <v>844</v>
+        <v>848</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="16" t="s">
-        <v>845</v>
+        <v>849</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="16" t="s">
-        <v>846</v>
+        <v>850</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="8" t="s">
-        <v>847</v>
+        <v>851</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="16" t="s">
-        <v>848</v>
+        <v>852</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="16" t="s">
-        <v>849</v>
+        <v>853</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="2" t="s">
-        <v>767</v>
+        <v>772</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="8" t="s">
-        <v>850</v>
+        <v>854</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="2" t="s">
-        <v>769</v>
+        <v>774</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="8" t="s">
-        <v>851</v>
+        <v>855</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="8" t="s">
-        <v>852</v>
+        <v>856</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="16" t="s">
-        <v>853</v>
+        <v>857</v>
       </c>
     </row>
   </sheetData>
@@ -44948,7 +45048,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -44960,57 +45060,57 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="2" t="s">
-        <v>743</v>
+        <v>748</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="16" t="s">
-        <v>854</v>
+        <v>858</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="16" t="s">
-        <v>855</v>
+        <v>859</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="16" t="s">
-        <v>856</v>
+        <v>860</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>750</v>
+        <v>755</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="8" t="s">
-        <v>857</v>
+        <v>861</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="16" t="s">
-        <v>858</v>
+        <v>862</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="8" t="s">
-        <v>859</v>
+        <v>863</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="s">
-        <v>767</v>
+        <v>772</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="8" t="s">
-        <v>860</v>
+        <v>864</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="16" t="s">
-        <v>861</v>
+        <v>865</v>
       </c>
     </row>
   </sheetData>
@@ -45028,7 +45128,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -45040,267 +45140,267 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="2" t="s">
-        <v>775</v>
+        <v>780</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="8" t="s">
-        <v>862</v>
+        <v>866</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="8" t="s">
-        <v>863</v>
+        <v>867</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="8" t="s">
-        <v>864</v>
+        <v>868</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="16" t="s">
-        <v>865</v>
+        <v>869</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="8" t="s">
-        <v>866</v>
+        <v>870</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="16" t="s">
-        <v>867</v>
+        <v>871</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="s">
-        <v>741</v>
+        <v>746</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="8" t="s">
-        <v>868</v>
+        <v>872</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="16" t="s">
-        <v>869</v>
+        <v>873</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="16" t="s">
-        <v>870</v>
+        <v>874</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="16" t="s">
-        <v>871</v>
+        <v>875</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="16" t="s">
-        <v>872</v>
+        <v>876</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="8" t="s">
-        <v>873</v>
+        <v>877</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="16" t="s">
-        <v>874</v>
+        <v>878</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="8" t="s">
-        <v>875</v>
+        <v>879</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="16" t="s">
-        <v>876</v>
+        <v>880</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="16" t="s">
-        <v>877</v>
+        <v>881</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="16" t="s">
-        <v>878</v>
+        <v>882</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="16" t="s">
-        <v>879</v>
+        <v>743</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="8" t="s">
-        <v>880</v>
+        <v>883</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="16" t="s">
-        <v>820</v>
+        <v>824</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="2" t="s">
-        <v>790</v>
+        <v>795</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="8" t="s">
-        <v>881</v>
+        <v>884</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="8" t="s">
-        <v>882</v>
+        <v>885</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="8" t="s">
-        <v>883</v>
+        <v>886</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="16" t="s">
-        <v>884</v>
+        <v>887</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="2" t="s">
-        <v>743</v>
+        <v>748</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="16" t="s">
-        <v>885</v>
+        <v>888</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="2" t="s">
-        <v>750</v>
+        <v>755</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="8" t="s">
-        <v>886</v>
+        <v>889</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="16" t="s">
-        <v>887</v>
+        <v>890</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="8" t="s">
-        <v>888</v>
+        <v>891</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="8" t="s">
-        <v>889</v>
+        <v>892</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="2" t="s">
-        <v>767</v>
+        <v>772</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="8" t="s">
-        <v>890</v>
+        <v>893</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="16" t="s">
-        <v>891</v>
+        <v>894</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="8" t="s">
-        <v>802</v>
+        <v>807</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="16" t="s">
-        <v>892</v>
+        <v>895</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="2" t="s">
-        <v>769</v>
+        <v>774</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="16" t="s">
-        <v>893</v>
+        <v>896</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="16" t="s">
-        <v>894</v>
+        <v>897</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="16" t="s">
-        <v>895</v>
+        <v>898</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="16" t="s">
-        <v>896</v>
+        <v>899</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="16" t="s">
-        <v>897</v>
+        <v>900</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="16" t="s">
-        <v>898</v>
+        <v>901</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="8" t="s">
-        <v>899</v>
+        <v>902</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="8" t="s">
-        <v>900</v>
+        <v>903</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="8" t="s">
-        <v>901</v>
+        <v>904</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="8" t="s">
-        <v>902</v>
+        <v>905</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="8" t="s">
-        <v>903</v>
+        <v>906</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="16" t="s">
-        <v>904</v>
+        <v>907</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="8" t="s">
-        <v>905</v>
+        <v>908</v>
       </c>
     </row>
   </sheetData>
@@ -45354,43 +45454,4 @@
   </hyperlinks>
   <drawing r:id="rId47"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="2" t="s">
-        <v>750</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="16" t="s">
-        <v>906</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="2" t="s">
-        <v>769</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="16" t="s">
-        <v>907</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink r:id="rId1" ref="A2"/>
-    <hyperlink r:id="rId2" ref="A4"/>
-  </hyperlinks>
-  <drawing r:id="rId3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
remove hf since chatbot arena update
</commit_message>
<xml_diff>
--- a/meta/Foundation Model Leaderboard Systems.xlsx
+++ b/meta/Foundation Model Leaderboard Systems.xlsx
@@ -77,7 +77,9 @@
       <text>
         <t xml:space="preserve">https://openlm.ai/chatbot-arena/
 	-Jimmy Chou
-https://chat.lmsys.org/
+https://chat.lmsys.org/?leaderboard
+	-Jimmy Chou
+https://huggingface.co/spaces/lmsys/chatbot-arena-leaderboard/discussions/31
 	-Jimmy Chou</t>
       </text>
     </comment>
@@ -973,31 +975,31 @@
 	-Jimmy Chou</t>
       </text>
     </comment>
-    <comment authorId="0" ref="E265">
+    <comment authorId="0" ref="E264">
       <text>
         <t xml:space="preserve">https://huggingface.co/spaces/FinancialSupport/open_ita_llm_leaderboard/discussions/4
 	-Jimmy Chou</t>
       </text>
     </comment>
-    <comment authorId="0" ref="H253">
+    <comment authorId="0" ref="H252">
       <text>
         <t xml:space="preserve">https://nexusflow.ai/blogs/ravenv2
 	-Jimmy Chou</t>
       </text>
     </comment>
-    <comment authorId="0" ref="A250">
+    <comment authorId="0" ref="A249">
       <text>
         <t xml:space="preserve">https://github.com/mesolitica/malaysian-stt-benchmarks
 	-Jimmy Chou</t>
       </text>
     </comment>
-    <comment authorId="0" ref="A248">
+    <comment authorId="0" ref="A247">
       <text>
         <t xml:space="preserve">https://github.com/mesolitica/llm-benchmarks
 	-Jimmy Chou</t>
       </text>
     </comment>
-    <comment authorId="0" ref="A249">
+    <comment authorId="0" ref="A248">
       <text>
         <t xml:space="preserve">https://github.com/mesolitica/embedding-benchmarks
 	-Jimmy Chou</t>
@@ -1083,7 +1085,7 @@
 	-Jimmy Chou</t>
       </text>
     </comment>
-    <comment authorId="0" ref="A251">
+    <comment authorId="0" ref="A250">
       <text>
         <t xml:space="preserve">https://github.com/allenai/natural-instructions
 	-Jimmy Chou</t>
@@ -1275,7 +1277,7 @@
 	-Jimmy Chou</t>
       </text>
     </comment>
-    <comment authorId="0" ref="F253">
+    <comment authorId="0" ref="F252">
       <text>
         <t xml:space="preserve">https://github.com/nexusflowai/NexusRaven/
 	-Jimmy Chou</t>
@@ -1293,13 +1295,13 @@
 	-Jimmy Chou</t>
       </text>
     </comment>
-    <comment authorId="0" ref="F248">
+    <comment authorId="0" ref="F247">
       <text>
         <t xml:space="preserve">https://github.com/mesolitica/llm-benchmarks
 	-Jimmy Chou</t>
       </text>
     </comment>
-    <comment authorId="0" ref="F265">
+    <comment authorId="0" ref="F264">
       <text>
         <t xml:space="preserve">https://github.com/C080/open-llm-ita-leaderboard
 	-Jimmy Chou</t>
@@ -1317,7 +1319,7 @@
 	-Jimmy Chou</t>
       </text>
     </comment>
-    <comment authorId="0" ref="D242">
+    <comment authorId="0" ref="D241">
       <text>
         <t xml:space="preserve">https://raw.githubusercontent.com/AI-Northstar-Tech/mteb-info/main/data/data.json
 	-Jimmy Chou</t>
@@ -1371,7 +1373,7 @@
 	-Jimmy Chou</t>
       </text>
     </comment>
-    <comment authorId="0" ref="F256">
+    <comment authorId="0" ref="F255">
       <text>
         <t xml:space="preserve">https://github.com/casmlab/NPHardEval
 	-Jimmy Chou</t>
@@ -1495,7 +1497,7 @@
 	-Jimmy Chou</t>
       </text>
     </comment>
-    <comment authorId="0" ref="F263">
+    <comment authorId="0" ref="F262">
       <text>
         <t xml:space="preserve">https://github.com/huggingface/open_asr_leaderboard
 	-Jimmy Chou</t>
@@ -1666,7 +1668,7 @@
 	-Jimmy Chou</t>
       </text>
     </comment>
-    <comment authorId="0" ref="F251">
+    <comment authorId="0" ref="F250">
       <text>
         <t xml:space="preserve">https://leaderboard.allenai.org/natural-instructions/submissions/public
 	-Jimmy Chou</t>
@@ -1800,7 +1802,7 @@
 	-Jimmy Chou</t>
       </text>
     </comment>
-    <comment authorId="0" ref="F247">
+    <comment authorId="0" ref="F246">
       <text>
         <t xml:space="preserve">https://huggingface.co/spaces/OpenGVLab/MVBench_Leaderboard
 	-Jimmy Chou
@@ -1917,7 +1919,7 @@
 	-Jimmy Chou</t>
       </text>
     </comment>
-    <comment authorId="0" ref="A267">
+    <comment authorId="0" ref="A266">
       <text>
         <t xml:space="preserve">https://huggingface.co/spaces/gsaivinay/open_llm_leaderboard
 	-Jimmy Chou</t>
@@ -2227,7 +2229,7 @@
 	-Jimmy Chou</t>
       </text>
     </comment>
-    <comment authorId="0" ref="F242">
+    <comment authorId="0" ref="F241">
       <text>
         <t xml:space="preserve">https://mteb.info
 	-Jimmy Chou</t>
@@ -2309,7 +2311,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2170" uniqueCount="921">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2171" uniqueCount="922">
   <si>
     <t>Leaderboard name</t>
   </si>
@@ -3407,7 +3409,7 @@
     <t>LMSYS Chatbot Arena Leaderboard</t>
   </si>
   <si>
-    <t>hf:Sortable Table+Scatter Plot+Bar Chart,ip:Sortable Table</t>
+    <t>ip:Sortable Table+Scatter Plot+Bar Chart</t>
   </si>
   <si>
     <t>4,5</t>
@@ -3644,184 +3646,184 @@
     <t>Artificial Analysis</t>
   </si>
   <si>
+    <t>MoleculeNet</t>
+  </si>
+  <si>
+    <t>Chemical Science</t>
+  </si>
+  <si>
+    <t>MRPC</t>
+  </si>
+  <si>
+    <t>IJCNLP</t>
+  </si>
+  <si>
+    <t>MSCOCO</t>
+  </si>
+  <si>
+    <t>MSRVTT</t>
+  </si>
+  <si>
+    <t>MSRVTT-QA</t>
+  </si>
+  <si>
+    <t>ACM-MM</t>
+  </si>
+  <si>
+    <t>MSTEB</t>
+  </si>
+  <si>
+    <t>Clibrain</t>
+  </si>
+  <si>
+    <t>MSVAMP</t>
+  </si>
+  <si>
+    <t>MSVD</t>
+  </si>
+  <si>
+    <t>MSVD-QA</t>
+  </si>
+  <si>
+    <t>MTEB</t>
+  </si>
+  <si>
+    <t>hf:Sortable Table,gh:Regular Table,ip:Sortable Table</t>
+  </si>
+  <si>
+    <t>gh,hf,ip,pwc</t>
+  </si>
+  <si>
+    <t>EACL</t>
+  </si>
+  <si>
+    <t>Hugging Face,Cohere</t>
+  </si>
+  <si>
+    <t>MultiRC</t>
+  </si>
+  <si>
+    <t>MusicCaps</t>
+  </si>
+  <si>
+    <t>MusicQA</t>
+  </si>
+  <si>
+    <t>MVBench</t>
+  </si>
+  <si>
+    <t>hf:Sortable Table,gh:Table Screenshot</t>
+  </si>
+  <si>
+    <t>Chinese Academy of Sciences,University of Chinese Academy of Sciences,Shanghai AI Laboratory,University of Hong Kong,Fudan University,Nanjing University</t>
+  </si>
+  <si>
+    <t>MY Malay LLM Leaderboard</t>
+  </si>
+  <si>
+    <t>Mesolitica</t>
+  </si>
+  <si>
+    <t>MY Malaysian Embedding Leaderboard</t>
+  </si>
+  <si>
+    <t>MY Malaysian Speech-to-Text Leaderboard</t>
+  </si>
+  <si>
+    <t>Natural Instructions (v2)</t>
+  </si>
+  <si>
+    <t>NExT-QA</t>
+  </si>
+  <si>
+    <t>Nexus Function Calling Leaderboard</t>
+  </si>
+  <si>
+    <t>hf:Sortable Table+Radar Chart</t>
+  </si>
+  <si>
+    <t>Nexusflow</t>
+  </si>
+  <si>
+    <t>NLVR</t>
+  </si>
+  <si>
+    <t>NoCaps</t>
+  </si>
+  <si>
+    <t>NPHardEval</t>
+  </si>
+  <si>
+    <t>University of Michigan Ann Arbor,Rutgers University</t>
+  </si>
+  <si>
+    <t>NPHardEval4V</t>
+  </si>
+  <si>
+    <t>University of Michigan,Rutgers University,Shandong University,Microsoft Research Asia</t>
+  </si>
+  <si>
+    <t>NQ</t>
+  </si>
+  <si>
+    <t>OCRBench</t>
+  </si>
+  <si>
+    <t>Huazhong University of Science and Technology,Microsoft,University of Science and Technology Beijing,Chinese Academy of Sciences,South China University of Technology</t>
+  </si>
+  <si>
+    <t>ODEX</t>
+  </si>
+  <si>
+    <t>Carnegie Mellon University,Inspired Cognition</t>
+  </si>
+  <si>
+    <t>OK-VQA</t>
+  </si>
+  <si>
+    <t>OmniBenchmark</t>
+  </si>
+  <si>
+    <t>Open ASR Leaderboard</t>
+  </si>
+  <si>
+    <t>Open Dutch LLM Evaluation Leaderboard</t>
+  </si>
+  <si>
+    <t>LATEX</t>
+  </si>
+  <si>
+    <t>Catholic University of Leuven</t>
+  </si>
+  <si>
+    <t>Open ITA LLM Leaderboard</t>
+  </si>
+  <si>
+    <t>Open Ko-LLM Leaderboard</t>
+  </si>
+  <si>
+    <t>Upstage</t>
+  </si>
+  <si>
+    <t>Open LLM Leaderboard</t>
+  </si>
+  <si>
+    <t>Open LLM Leaderboard (GPT)</t>
+  </si>
+  <si>
+    <t>Open Medical-LLM Leaderboard</t>
+  </si>
+  <si>
+    <t>Nature</t>
+  </si>
+  <si>
+    <t>Google,National Library of Medicine,Google DeepMind</t>
+  </si>
+  <si>
+    <t>Open MLLM Leaderboard</t>
+  </si>
+  <si>
     <t>OPEN MOE LLM Leaderboard</t>
-  </si>
-  <si>
-    <t>MoleculeNet</t>
-  </si>
-  <si>
-    <t>Chemical Science</t>
-  </si>
-  <si>
-    <t>MRPC</t>
-  </si>
-  <si>
-    <t>IJCNLP</t>
-  </si>
-  <si>
-    <t>MSCOCO</t>
-  </si>
-  <si>
-    <t>MSRVTT</t>
-  </si>
-  <si>
-    <t>MSRVTT-QA</t>
-  </si>
-  <si>
-    <t>ACM-MM</t>
-  </si>
-  <si>
-    <t>MSTEB</t>
-  </si>
-  <si>
-    <t>Clibrain</t>
-  </si>
-  <si>
-    <t>MSVAMP</t>
-  </si>
-  <si>
-    <t>MSVD</t>
-  </si>
-  <si>
-    <t>MSVD-QA</t>
-  </si>
-  <si>
-    <t>MTEB</t>
-  </si>
-  <si>
-    <t>hf:Sortable Table,gh:Regular Table,ip:Sortable Table</t>
-  </si>
-  <si>
-    <t>gh,hf,ip,pwc</t>
-  </si>
-  <si>
-    <t>EACL</t>
-  </si>
-  <si>
-    <t>Hugging Face,Cohere</t>
-  </si>
-  <si>
-    <t>MultiRC</t>
-  </si>
-  <si>
-    <t>MusicCaps</t>
-  </si>
-  <si>
-    <t>MusicQA</t>
-  </si>
-  <si>
-    <t>MVBench</t>
-  </si>
-  <si>
-    <t>hf:Sortable Table,gh:Table Screenshot</t>
-  </si>
-  <si>
-    <t>Chinese Academy of Sciences,University of Chinese Academy of Sciences,Shanghai AI Laboratory,University of Hong Kong,Fudan University,Nanjing University</t>
-  </si>
-  <si>
-    <t>MY Malay LLM Leaderboard</t>
-  </si>
-  <si>
-    <t>Mesolitica</t>
-  </si>
-  <si>
-    <t>MY Malaysian Embedding Leaderboard</t>
-  </si>
-  <si>
-    <t>MY Malaysian Speech-to-Text Leaderboard</t>
-  </si>
-  <si>
-    <t>Natural Instructions (v2)</t>
-  </si>
-  <si>
-    <t>NExT-QA</t>
-  </si>
-  <si>
-    <t>Nexus Function Calling Leaderboard</t>
-  </si>
-  <si>
-    <t>hf:Sortable Table+Radar Chart</t>
-  </si>
-  <si>
-    <t>Nexusflow</t>
-  </si>
-  <si>
-    <t>NLVR</t>
-  </si>
-  <si>
-    <t>NoCaps</t>
-  </si>
-  <si>
-    <t>NPHardEval</t>
-  </si>
-  <si>
-    <t>University of Michigan Ann Arbor,Rutgers University</t>
-  </si>
-  <si>
-    <t>NPHardEval4V</t>
-  </si>
-  <si>
-    <t>University of Michigan,Rutgers University,Shandong University,Microsoft Research Asia</t>
-  </si>
-  <si>
-    <t>NQ</t>
-  </si>
-  <si>
-    <t>OCRBench</t>
-  </si>
-  <si>
-    <t>Huazhong University of Science and Technology,Microsoft,University of Science and Technology Beijing,Chinese Academy of Sciences,South China University of Technology</t>
-  </si>
-  <si>
-    <t>ODEX</t>
-  </si>
-  <si>
-    <t>Carnegie Mellon University,Inspired Cognition</t>
-  </si>
-  <si>
-    <t>OK-VQA</t>
-  </si>
-  <si>
-    <t>OmniBenchmark</t>
-  </si>
-  <si>
-    <t>Open ASR Leaderboard</t>
-  </si>
-  <si>
-    <t>Open Dutch LLM Evaluation Leaderboard</t>
-  </si>
-  <si>
-    <t>LATEX</t>
-  </si>
-  <si>
-    <t>Catholic University of Leuven</t>
-  </si>
-  <si>
-    <t>Open ITA LLM Leaderboard</t>
-  </si>
-  <si>
-    <t>Open Ko-LLM Leaderboard</t>
-  </si>
-  <si>
-    <t>Upstage</t>
-  </si>
-  <si>
-    <t>Open LLM Leaderboard</t>
-  </si>
-  <si>
-    <t>Open LLM Leaderboard (GPT)</t>
-  </si>
-  <si>
-    <t>Open Medical-LLM Leaderboard</t>
-  </si>
-  <si>
-    <t>Nature</t>
-  </si>
-  <si>
-    <t>Google,National Library of Medicine,Google DeepMind</t>
-  </si>
-  <si>
-    <t>Open MLLM Leaderboard</t>
   </si>
   <si>
     <t>Open Multilingual LLM Evaluation Leaderboard</t>
@@ -4923,6 +4925,9 @@
   </si>
   <si>
     <t>https://github.com/OpenLMLab/LEval/issues/10</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/lmsys/chatbot-arena-leaderboard/discussions/31</t>
   </si>
   <si>
     <t>https://github.com/stanford-crfm/helm/issues/2386</t>
@@ -9033,7 +9038,7 @@
         <v>366</v>
       </c>
       <c r="F189" s="2" t="s">
-        <v>44</v>
+        <v>14</v>
       </c>
       <c r="G189" s="2" t="s">
         <v>15</v>
@@ -9871,46 +9876,36 @@
       <c r="A232" s="8" t="s">
         <v>444</v>
       </c>
-      <c r="C232" s="2" t="s">
-        <v>39</v>
-      </c>
+      <c r="C232" s="2"/>
       <c r="D232" s="2"/>
-      <c r="E232" s="2">
-        <v>4.0</v>
-      </c>
       <c r="F232" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="G232" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H232" s="7"/>
-      <c r="I232" s="2" t="s">
-        <v>58</v>
+        <v>10</v>
+      </c>
+      <c r="H232" s="7" t="s">
+        <v>445</v>
       </c>
     </row>
     <row r="233">
       <c r="A233" s="8" t="s">
-        <v>445</v>
-      </c>
-      <c r="C233" s="2"/>
-      <c r="D233" s="2"/>
+        <v>446</v>
+      </c>
       <c r="F233" s="2" t="s">
         <v>10</v>
       </c>
       <c r="H233" s="7" t="s">
-        <v>446</v>
-      </c>
+        <v>447</v>
+      </c>
+      <c r="I233" s="2"/>
     </row>
     <row r="234">
       <c r="A234" s="8" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="F234" s="2" t="s">
         <v>10</v>
       </c>
       <c r="H234" s="7" t="s">
-        <v>448</v>
+        <v>11</v>
       </c>
       <c r="I234" s="2"/>
     </row>
@@ -9922,7 +9917,7 @@
         <v>10</v>
       </c>
       <c r="H235" s="7" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="I235" s="2"/>
     </row>
@@ -9934,60 +9929,60 @@
         <v>10</v>
       </c>
       <c r="H236" s="7" t="s">
-        <v>25</v>
+        <v>451</v>
       </c>
       <c r="I236" s="2"/>
     </row>
     <row r="237">
       <c r="A237" s="8" t="s">
-        <v>451</v>
+        <v>452</v>
+      </c>
+      <c r="C237" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D237" s="2"/>
+      <c r="E237" s="2">
+        <v>2.0</v>
       </c>
       <c r="F237" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="H237" s="7" t="s">
-        <v>452</v>
-      </c>
-      <c r="I237" s="2"/>
+        <v>40</v>
+      </c>
+      <c r="H237" s="7"/>
+      <c r="I237" s="2" t="s">
+        <v>453</v>
+      </c>
     </row>
     <row r="238">
       <c r="A238" s="8" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="C238" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="D238" s="2"/>
+        <v>20</v>
+      </c>
       <c r="E238" s="2">
         <v>2.0</v>
       </c>
       <c r="F238" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="H238" s="7"/>
+        <v>21</v>
+      </c>
+      <c r="H238" s="7" t="s">
+        <v>32</v>
+      </c>
       <c r="I238" s="2" t="s">
-        <v>454</v>
+        <v>406</v>
       </c>
     </row>
     <row r="239">
       <c r="A239" s="8" t="s">
         <v>455</v>
       </c>
-      <c r="C239" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E239" s="2">
-        <v>2.0</v>
-      </c>
       <c r="F239" s="2" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="H239" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="I239" s="2" t="s">
-        <v>406</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="I239" s="2"/>
     </row>
     <row r="240">
       <c r="A240" s="8" t="s">
@@ -9997,7 +9992,7 @@
         <v>10</v>
       </c>
       <c r="H240" s="7" t="s">
-        <v>60</v>
+        <v>451</v>
       </c>
       <c r="I240" s="2"/>
     </row>
@@ -10005,39 +10000,39 @@
       <c r="A241" s="8" t="s">
         <v>457</v>
       </c>
+      <c r="C241" s="2" t="s">
+        <v>458</v>
+      </c>
+      <c r="D241" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="E241" s="2">
+        <v>10.0</v>
+      </c>
       <c r="F241" s="2" t="s">
-        <v>10</v>
+        <v>459</v>
+      </c>
+      <c r="G241" s="2" t="s">
+        <v>15</v>
       </c>
       <c r="H241" s="7" t="s">
-        <v>452</v>
-      </c>
-      <c r="I241" s="2"/>
+        <v>460</v>
+      </c>
+      <c r="I241" s="2" t="s">
+        <v>461</v>
+      </c>
     </row>
     <row r="242">
       <c r="A242" s="8" t="s">
-        <v>458</v>
-      </c>
-      <c r="C242" s="2" t="s">
-        <v>459</v>
-      </c>
-      <c r="D242" s="2" t="s">
-        <v>324</v>
-      </c>
-      <c r="E242" s="2">
-        <v>10.0</v>
+        <v>462</v>
       </c>
       <c r="F242" s="2" t="s">
-        <v>460</v>
-      </c>
-      <c r="G242" s="2" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="H242" s="7" t="s">
-        <v>461</v>
-      </c>
-      <c r="I242" s="2" t="s">
-        <v>462</v>
-      </c>
+        <v>102</v>
+      </c>
+      <c r="I242" s="2"/>
     </row>
     <row r="243">
       <c r="A243" s="8" t="s">
@@ -10047,13 +10042,12 @@
         <v>10</v>
       </c>
       <c r="H243" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="I243" s="2"/>
+        <v>32</v>
+      </c>
     </row>
     <row r="244">
       <c r="A244" s="8" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="F244" s="2" t="s">
         <v>10</v>
@@ -10066,6 +10060,8 @@
       <c r="A245" s="8" t="s">
         <v>464</v>
       </c>
+      <c r="C245" s="2"/>
+      <c r="D245" s="2"/>
       <c r="F245" s="2" t="s">
         <v>10</v>
       </c>
@@ -10077,41 +10073,50 @@
       <c r="A246" s="8" t="s">
         <v>465</v>
       </c>
-      <c r="C246" s="2"/>
-      <c r="D246" s="2"/>
+      <c r="C246" s="2" t="s">
+        <v>466</v>
+      </c>
+      <c r="D246" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E246" s="2">
+        <v>7.0</v>
+      </c>
       <c r="F246" s="2" t="s">
-        <v>10</v>
+        <v>173</v>
       </c>
       <c r="H246" s="7" t="s">
         <v>32</v>
       </c>
+      <c r="I246" s="2" t="s">
+        <v>467</v>
+      </c>
     </row>
     <row r="247">
       <c r="A247" s="8" t="s">
-        <v>466</v>
+        <v>468</v>
       </c>
       <c r="C247" s="2" t="s">
-        <v>467</v>
-      </c>
-      <c r="D247" s="2" t="s">
-        <v>13</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="D247" s="2"/>
       <c r="E247" s="2">
-        <v>7.0</v>
+        <v>2.0</v>
       </c>
       <c r="F247" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="H247" s="7" t="s">
-        <v>32</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="G247" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H247" s="7"/>
       <c r="I247" s="2" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
     </row>
     <row r="248">
       <c r="A248" s="8" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="C248" s="2" t="s">
         <v>39</v>
@@ -10126,9 +10131,9 @@
       <c r="G248" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="H248" s="7"/>
+      <c r="H248" s="10"/>
       <c r="I248" s="2" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="249">
@@ -10145,12 +10150,9 @@
       <c r="F249" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="G249" s="2" t="s">
-        <v>15</v>
-      </c>
       <c r="H249" s="10"/>
       <c r="I249" s="2" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="250">
@@ -10158,77 +10160,69 @@
         <v>472</v>
       </c>
       <c r="C250" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="D250" s="2"/>
+        <v>12</v>
+      </c>
+      <c r="D250" s="2" t="s">
+        <v>13</v>
+      </c>
       <c r="E250" s="2">
-        <v>2.0</v>
+        <v>6.0</v>
       </c>
       <c r="F250" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="H250" s="10"/>
+        <v>14</v>
+      </c>
+      <c r="G250" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H250" s="7" t="s">
+        <v>60</v>
+      </c>
       <c r="I250" s="2" t="s">
-        <v>470</v>
+        <v>16</v>
       </c>
     </row>
     <row r="251">
       <c r="A251" s="8" t="s">
         <v>473</v>
       </c>
-      <c r="C251" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D251" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E251" s="2">
-        <v>6.0</v>
-      </c>
       <c r="F251" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G251" s="2" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="H251" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="I251" s="2" t="s">
-        <v>16</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="I251" s="2"/>
     </row>
     <row r="252">
       <c r="A252" s="8" t="s">
         <v>474</v>
       </c>
+      <c r="C252" s="2" t="s">
+        <v>475</v>
+      </c>
+      <c r="D252" s="2"/>
+      <c r="E252" s="2">
+        <v>2.0</v>
+      </c>
       <c r="F252" s="2" t="s">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="H252" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="I252" s="2"/>
+        <v>270</v>
+      </c>
+      <c r="I252" s="2" t="s">
+        <v>476</v>
+      </c>
     </row>
     <row r="253">
       <c r="A253" s="8" t="s">
-        <v>475</v>
-      </c>
-      <c r="C253" s="2" t="s">
-        <v>476</v>
-      </c>
-      <c r="D253" s="2"/>
-      <c r="E253" s="2">
-        <v>2.0</v>
+        <v>477</v>
       </c>
       <c r="F253" s="2" t="s">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="H253" s="7" t="s">
-        <v>270</v>
-      </c>
-      <c r="I253" s="2" t="s">
-        <v>477</v>
+        <v>60</v>
       </c>
     </row>
     <row r="254">
@@ -10239,124 +10233,125 @@
         <v>10</v>
       </c>
       <c r="H254" s="7" t="s">
-        <v>60</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="I254" s="2"/>
     </row>
     <row r="255">
       <c r="A255" s="8" t="s">
         <v>479</v>
       </c>
+      <c r="C255" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="D255" s="2"/>
+      <c r="E255" s="2">
+        <v>2.0</v>
+      </c>
       <c r="F255" s="2" t="s">
-        <v>10</v>
+        <v>173</v>
+      </c>
+      <c r="G255" s="2" t="s">
+        <v>15</v>
       </c>
       <c r="H255" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="I255" s="2"/>
+        <v>32</v>
+      </c>
+      <c r="I255" s="2" t="s">
+        <v>480</v>
+      </c>
     </row>
     <row r="256">
       <c r="A256" s="8" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="C256" s="2" t="s">
-        <v>172</v>
+        <v>20</v>
       </c>
       <c r="D256" s="2"/>
       <c r="E256" s="2">
         <v>2.0</v>
       </c>
       <c r="F256" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="G256" s="2" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="H256" s="7" t="s">
         <v>32</v>
       </c>
       <c r="I256" s="2" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
     </row>
     <row r="257">
       <c r="A257" s="8" t="s">
-        <v>482</v>
-      </c>
-      <c r="C257" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D257" s="2"/>
-      <c r="E257" s="2">
-        <v>2.0</v>
+        <v>483</v>
       </c>
       <c r="F257" s="2" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="H257" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="I257" s="2" t="s">
-        <v>483</v>
-      </c>
+        <v>163</v>
+      </c>
+      <c r="I257" s="2"/>
     </row>
     <row r="258">
       <c r="A258" s="8" t="s">
         <v>484</v>
       </c>
+      <c r="C258" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D258" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E258" s="2">
+        <v>7.0</v>
+      </c>
       <c r="F258" s="2" t="s">
-        <v>10</v>
+        <v>40</v>
+      </c>
+      <c r="G258" s="2" t="s">
+        <v>15</v>
       </c>
       <c r="H258" s="7" t="s">
-        <v>163</v>
-      </c>
-      <c r="I258" s="2"/>
+        <v>32</v>
+      </c>
+      <c r="I258" s="2" t="s">
+        <v>485</v>
+      </c>
     </row>
     <row r="259">
       <c r="A259" s="8" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="C259" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="D259" s="2" t="s">
-        <v>13</v>
-      </c>
+        <v>81</v>
+      </c>
+      <c r="D259" s="2"/>
       <c r="E259" s="2">
-        <v>7.0</v>
+        <v>2.0</v>
       </c>
       <c r="F259" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="G259" s="2" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="H259" s="7" t="s">
-        <v>32</v>
+        <v>97</v>
       </c>
       <c r="I259" s="2" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
     </row>
     <row r="260">
       <c r="A260" s="8" t="s">
-        <v>487</v>
-      </c>
-      <c r="C260" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="D260" s="2"/>
-      <c r="E260" s="2">
-        <v>2.0</v>
+        <v>488</v>
       </c>
       <c r="F260" s="2" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="H260" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="I260" s="2" t="s">
-        <v>488</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="I260" s="2"/>
     </row>
     <row r="261">
       <c r="A261" s="8" t="s">
@@ -10366,7 +10361,7 @@
         <v>10</v>
       </c>
       <c r="H261" s="7" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="I261" s="2"/>
     </row>
@@ -10374,24 +10369,38 @@
       <c r="A262" s="8" t="s">
         <v>490</v>
       </c>
+      <c r="C262" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D262" s="2"/>
+      <c r="E262" s="2">
+        <v>4.0</v>
+      </c>
       <c r="F262" s="2" t="s">
-        <v>10</v>
+        <v>40</v>
+      </c>
+      <c r="G262" s="2" t="s">
+        <v>15</v>
       </c>
       <c r="H262" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="I262" s="2"/>
+        <v>32</v>
+      </c>
+      <c r="I262" s="2" t="s">
+        <v>353</v>
+      </c>
     </row>
     <row r="263">
       <c r="A263" s="8" t="s">
         <v>491</v>
       </c>
       <c r="C263" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="D263" s="2"/>
+        <v>266</v>
+      </c>
+      <c r="D263" s="2" t="s">
+        <v>492</v>
+      </c>
       <c r="E263" s="2">
-        <v>4.0</v>
+        <v>2.0</v>
       </c>
       <c r="F263" s="2" t="s">
         <v>40</v>
@@ -10403,33 +10412,28 @@
         <v>32</v>
       </c>
       <c r="I263" s="2" t="s">
-        <v>353</v>
+        <v>493</v>
       </c>
     </row>
     <row r="264">
       <c r="A264" s="8" t="s">
-        <v>492</v>
+        <v>494</v>
       </c>
       <c r="C264" s="2" t="s">
-        <v>266</v>
+        <v>39</v>
       </c>
       <c r="D264" s="2" t="s">
-        <v>493</v>
+        <v>13</v>
       </c>
       <c r="E264" s="2">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
       <c r="F264" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="G264" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H264" s="7" t="s">
-        <v>32</v>
-      </c>
+      <c r="H264" s="7"/>
       <c r="I264" s="2" t="s">
-        <v>494</v>
+        <v>58</v>
       </c>
     </row>
     <row r="265">
@@ -10439,26 +10443,27 @@
       <c r="C265" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D265" s="2" t="s">
-        <v>13</v>
-      </c>
+      <c r="D265" s="2"/>
       <c r="E265" s="2">
         <v>4.0</v>
       </c>
       <c r="F265" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="H265" s="7"/>
+      <c r="G265" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H265" s="10"/>
       <c r="I265" s="2" t="s">
-        <v>58</v>
+        <v>496</v>
       </c>
     </row>
     <row r="266">
       <c r="A266" s="8" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="C266" s="2" t="s">
-        <v>39</v>
+        <v>88</v>
       </c>
       <c r="D266" s="2"/>
       <c r="E266" s="2">
@@ -10472,7 +10477,7 @@
       </c>
       <c r="H266" s="10"/>
       <c r="I266" s="2" t="s">
-        <v>497</v>
+        <v>353</v>
       </c>
     </row>
     <row r="267">
@@ -10480,7 +10485,7 @@
         <v>498</v>
       </c>
       <c r="C267" s="2" t="s">
-        <v>88</v>
+        <v>39</v>
       </c>
       <c r="D267" s="2"/>
       <c r="E267" s="2">
@@ -10494,7 +10499,7 @@
       </c>
       <c r="H267" s="10"/>
       <c r="I267" s="2" t="s">
-        <v>353</v>
+        <v>58</v>
       </c>
     </row>
     <row r="268">
@@ -10514,21 +10519,23 @@
       <c r="G268" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="H268" s="10"/>
+      <c r="H268" s="7" t="s">
+        <v>500</v>
+      </c>
       <c r="I268" s="2" t="s">
-        <v>58</v>
+        <v>501</v>
       </c>
     </row>
     <row r="269">
       <c r="A269" s="8" t="s">
-        <v>500</v>
+        <v>502</v>
       </c>
       <c r="C269" s="2" t="s">
         <v>39</v>
       </c>
       <c r="D269" s="2"/>
       <c r="E269" s="2">
-        <v>4.0</v>
+        <v>2.0</v>
       </c>
       <c r="F269" s="2" t="s">
         <v>40</v>
@@ -10536,11 +10543,9 @@
       <c r="G269" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="H269" s="7" t="s">
-        <v>501</v>
-      </c>
+      <c r="H269" s="7"/>
       <c r="I269" s="2" t="s">
-        <v>502</v>
+        <v>58</v>
       </c>
     </row>
     <row r="270">
@@ -10552,7 +10557,7 @@
       </c>
       <c r="D270" s="2"/>
       <c r="E270" s="2">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
       <c r="F270" s="2" t="s">
         <v>40</v>
@@ -12582,7 +12587,7 @@
         <v>21</v>
       </c>
       <c r="H370" s="7" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="I370" s="2" t="s">
         <v>651</v>
@@ -16453,7 +16458,7 @@
     </row>
     <row r="2">
       <c r="A2" s="16" t="s">
-        <v>919</v>
+        <v>920</v>
       </c>
     </row>
     <row r="3">
@@ -16463,7 +16468,7 @@
     </row>
     <row r="4">
       <c r="A4" s="16" t="s">
-        <v>920</v>
+        <v>921</v>
       </c>
     </row>
   </sheetData>
@@ -45223,23 +45228,23 @@
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="2" t="s">
+      <c r="A17" s="8" t="s">
+        <v>864</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="2" t="s">
         <v>781</v>
       </c>
     </row>
-    <row r="18">
-      <c r="A18" s="8" t="s">
-        <v>864</v>
-      </c>
-    </row>
     <row r="19">
-      <c r="A19" s="2" t="s">
+      <c r="A19" s="8" t="s">
+        <v>865</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="2" t="s">
         <v>783</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="8" t="s">
-        <v>865</v>
       </c>
     </row>
     <row r="21">
@@ -45248,8 +45253,13 @@
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="16" t="s">
+      <c r="A22" s="8" t="s">
         <v>867</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="16" t="s">
+        <v>868</v>
       </c>
     </row>
   </sheetData>
@@ -45266,12 +45276,13 @@
     <hyperlink r:id="rId10" ref="A14"/>
     <hyperlink r:id="rId11" ref="A15"/>
     <hyperlink r:id="rId12" ref="A16"/>
-    <hyperlink r:id="rId13" ref="A18"/>
-    <hyperlink r:id="rId14" ref="A20"/>
+    <hyperlink r:id="rId13" ref="A17"/>
+    <hyperlink r:id="rId14" ref="A19"/>
     <hyperlink r:id="rId15" ref="A21"/>
     <hyperlink r:id="rId16" ref="A22"/>
+    <hyperlink r:id="rId17" ref="A23"/>
   </hyperlinks>
-  <drawing r:id="rId17"/>
+  <drawing r:id="rId18"/>
 </worksheet>
 </file>
 
@@ -45292,17 +45303,17 @@
     </row>
     <row r="2">
       <c r="A2" s="16" t="s">
-        <v>868</v>
+        <v>869</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="16" t="s">
-        <v>869</v>
+        <v>870</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="16" t="s">
-        <v>870</v>
+        <v>871</v>
       </c>
     </row>
     <row r="5">
@@ -45312,17 +45323,17 @@
     </row>
     <row r="6">
       <c r="A6" s="8" t="s">
-        <v>871</v>
+        <v>872</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="16" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="8" t="s">
-        <v>873</v>
+        <v>874</v>
       </c>
     </row>
     <row r="9">
@@ -45332,12 +45343,12 @@
     </row>
     <row r="10">
       <c r="A10" s="8" t="s">
-        <v>874</v>
+        <v>875</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="16" t="s">
-        <v>875</v>
+        <v>876</v>
       </c>
     </row>
   </sheetData>
@@ -45372,27 +45383,27 @@
     </row>
     <row r="2">
       <c r="A2" s="8" t="s">
-        <v>876</v>
+        <v>877</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="8" t="s">
-        <v>877</v>
+        <v>878</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="8" t="s">
-        <v>878</v>
+        <v>879</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="16" t="s">
-        <v>879</v>
+        <v>880</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="8" t="s">
-        <v>880</v>
+        <v>881</v>
       </c>
     </row>
     <row r="7">
@@ -45407,57 +45418,57 @@
     </row>
     <row r="9">
       <c r="A9" s="8" t="s">
-        <v>881</v>
+        <v>882</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="16" t="s">
-        <v>882</v>
+        <v>883</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="16" t="s">
-        <v>883</v>
+        <v>884</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="16" t="s">
-        <v>884</v>
+        <v>885</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="16" t="s">
-        <v>885</v>
+        <v>886</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="8" t="s">
-        <v>886</v>
+        <v>887</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="16" t="s">
-        <v>887</v>
+        <v>888</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="8" t="s">
-        <v>888</v>
+        <v>889</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="16" t="s">
-        <v>889</v>
+        <v>890</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="16" t="s">
-        <v>890</v>
+        <v>891</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="16" t="s">
-        <v>891</v>
+        <v>892</v>
       </c>
     </row>
     <row r="20">
@@ -45467,7 +45478,7 @@
     </row>
     <row r="21">
       <c r="A21" s="8" t="s">
-        <v>892</v>
+        <v>893</v>
       </c>
     </row>
     <row r="22">
@@ -45482,22 +45493,22 @@
     </row>
     <row r="24">
       <c r="A24" s="8" t="s">
-        <v>893</v>
+        <v>894</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="8" t="s">
-        <v>894</v>
+        <v>895</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="8" t="s">
-        <v>895</v>
+        <v>896</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="16" t="s">
-        <v>896</v>
+        <v>897</v>
       </c>
     </row>
     <row r="28">
@@ -45507,7 +45518,7 @@
     </row>
     <row r="29">
       <c r="A29" s="16" t="s">
-        <v>897</v>
+        <v>898</v>
       </c>
     </row>
     <row r="30">
@@ -45517,22 +45528,22 @@
     </row>
     <row r="31">
       <c r="A31" s="8" t="s">
-        <v>898</v>
+        <v>899</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="16" t="s">
-        <v>899</v>
+        <v>900</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="8" t="s">
-        <v>900</v>
+        <v>901</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="8" t="s">
-        <v>901</v>
+        <v>902</v>
       </c>
     </row>
     <row r="35">
@@ -45542,12 +45553,12 @@
     </row>
     <row r="36">
       <c r="A36" s="8" t="s">
-        <v>902</v>
+        <v>903</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="16" t="s">
-        <v>903</v>
+        <v>904</v>
       </c>
     </row>
     <row r="38">
@@ -45557,7 +45568,7 @@
     </row>
     <row r="39">
       <c r="A39" s="16" t="s">
-        <v>904</v>
+        <v>905</v>
       </c>
     </row>
     <row r="40">
@@ -45567,72 +45578,72 @@
     </row>
     <row r="41">
       <c r="A41" s="16" t="s">
-        <v>905</v>
+        <v>906</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="16" t="s">
-        <v>906</v>
+        <v>907</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="16" t="s">
-        <v>907</v>
+        <v>908</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="16" t="s">
-        <v>908</v>
+        <v>909</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="16" t="s">
-        <v>909</v>
+        <v>910</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="16" t="s">
-        <v>910</v>
+        <v>911</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="8" t="s">
-        <v>911</v>
+        <v>912</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="8" t="s">
-        <v>912</v>
+        <v>913</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="8" t="s">
-        <v>913</v>
+        <v>914</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="8" t="s">
-        <v>914</v>
+        <v>915</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="8" t="s">
-        <v>915</v>
+        <v>916</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="16" t="s">
-        <v>916</v>
+        <v>917</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="8" t="s">
-        <v>917</v>
+        <v>918</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="8" t="s">
-        <v>918</v>
+        <v>919</v>
       </c>
     </row>
   </sheetData>

</xml_diff>